<commit_message>
Cambios en transportistas modulo InfractionDetail
</commit_message>
<xml_diff>
--- a/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/VehicleInfractionsDetails.xlsx
+++ b/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/VehicleInfractionsDetails.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias Alfano\Source\Repos\Logictracker 4.0\Logictracker\Logictracker\src\Web\Logictracker\Logictracker.Web\ExcelTemplate\Logictracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,29 +15,30 @@
     <sheet name="Informe" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Informe!$A$8:$J$8</definedName>
-    <definedName name="CALIFICACION">Informe!$C$8</definedName>
-    <definedName name="CALIFICACION_STR">Informe!$U$8</definedName>
-    <definedName name="CHOFER">Informe!$D$8</definedName>
-    <definedName name="Desde">Informe!$C$5</definedName>
-    <definedName name="DURACION">Informe!$G$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Informe!$A$8:$K$8</definedName>
+    <definedName name="CALIFICACION">Informe!$D$8</definedName>
+    <definedName name="CALIFICACION_STR">Informe!$V$8</definedName>
+    <definedName name="CHOFER">Informe!$E$8</definedName>
+    <definedName name="Desde">Informe!$D$5</definedName>
+    <definedName name="DURACION">Informe!$H$8</definedName>
     <definedName name="Empleado">Informe!#REF!</definedName>
-    <definedName name="ESQUINA">Informe!$E$8</definedName>
-    <definedName name="EXCESO">Informe!$I$8</definedName>
-    <definedName name="Hasta">Informe!$C$6</definedName>
-    <definedName name="INICIO">Informe!$F$8</definedName>
+    <definedName name="ESQUINA">Informe!$F$8</definedName>
+    <definedName name="EXCESO">Informe!$J$8</definedName>
+    <definedName name="Hasta">Informe!$D$6</definedName>
+    <definedName name="INICIO">Informe!$G$8</definedName>
     <definedName name="PARENTI03">Informe!$A$8</definedName>
-    <definedName name="PICO">Informe!$H$8</definedName>
-    <definedName name="PONDERACION">Informe!$J$8</definedName>
-    <definedName name="TIPO_INFRACCION">Informe!$B$8</definedName>
-    <definedName name="Titulo">Informe!$C$1</definedName>
+    <definedName name="PARENTI07">Informe!$B$8</definedName>
+    <definedName name="PICO">Informe!$I$8</definedName>
+    <definedName name="PONDERACION">Informe!$K$8</definedName>
+    <definedName name="TIPO_INFRACCION">Informe!$C$8</definedName>
+    <definedName name="Titulo">Informe!$D$1</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Desde: </t>
   </si>
@@ -76,6 +77,9 @@
   </si>
   <si>
     <t>Tipo de infracción</t>
+  </si>
+  <si>
+    <t>Transportista</t>
   </si>
 </sst>
 </file>
@@ -654,11 +658,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -733,8 +737,8 @@
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1552574</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>211740</xdr:rowOff>
     </xdr:to>
@@ -1062,686 +1066,691 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U196"/>
+  <dimension ref="A1:V196"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.140625" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="1" max="2" width="18.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.140625" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="C1" s="10" t="s">
+    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="L1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
-      <c r="I2" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="1"/>
       <c r="J2" s="2"/>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I3" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J3" s="2"/>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I4" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J4" s="2"/>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F7" s="15"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="D8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="E8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="G8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="H8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="J8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G31" s="4"/>
-    </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G34" s="4"/>
-    </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G36" s="4"/>
-    </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G37" s="4"/>
-    </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G38" s="4"/>
-    </row>
-    <row r="39" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G39" s="4"/>
-    </row>
-    <row r="40" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G40" s="4"/>
-    </row>
-    <row r="41" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G41" s="4"/>
-    </row>
-    <row r="42" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G42" s="4"/>
-    </row>
-    <row r="43" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G43" s="4"/>
-    </row>
-    <row r="44" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G44" s="4"/>
-    </row>
-    <row r="45" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G45" s="4"/>
-    </row>
-    <row r="46" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G46" s="4"/>
-    </row>
-    <row r="47" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G47" s="4"/>
-    </row>
-    <row r="48" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G48" s="4"/>
-    </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G49" s="4"/>
-    </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G50" s="4"/>
-    </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G51" s="4"/>
-    </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G52" s="4"/>
-    </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G53" s="4"/>
-    </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G54" s="4"/>
-    </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G55" s="4"/>
-    </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G56" s="4"/>
-    </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G57" s="4"/>
-    </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G58" s="4"/>
-    </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G59" s="4"/>
-    </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G60" s="4"/>
-    </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G61" s="4"/>
-    </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G62" s="4"/>
-    </row>
-    <row r="63" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G63" s="4"/>
-    </row>
-    <row r="64" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G64" s="4"/>
-    </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G65" s="4"/>
-    </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G66" s="4"/>
-    </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G67" s="4"/>
-    </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G68" s="4"/>
-    </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G69" s="4"/>
-    </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G70" s="4"/>
-    </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G71" s="4"/>
-    </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G72" s="4"/>
-    </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G73" s="4"/>
-    </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G74" s="4"/>
-    </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G75" s="4"/>
-    </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G76" s="4"/>
-    </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G77" s="4"/>
-    </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G78" s="4"/>
-    </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G79" s="4"/>
-    </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G80" s="4"/>
-    </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G81" s="4"/>
-    </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G82" s="4"/>
-    </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G83" s="4"/>
-    </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G84" s="4"/>
-    </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G85" s="4"/>
-    </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G86" s="4"/>
-    </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G87" s="4"/>
-    </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G88" s="4"/>
-    </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G89" s="4"/>
-    </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G90" s="4"/>
-    </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G91" s="4"/>
-    </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G92" s="4"/>
-    </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G93" s="4"/>
-    </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G94" s="4"/>
-    </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G95" s="4"/>
-    </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G96" s="4"/>
-    </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G97" s="4"/>
-    </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G98" s="4"/>
-    </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G99" s="4"/>
-    </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G100" s="4"/>
-    </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G101" s="4"/>
-    </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G102" s="4"/>
-    </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G103" s="4"/>
-    </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G104" s="4"/>
-    </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G105" s="4"/>
-    </row>
-    <row r="106" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G106" s="4"/>
-    </row>
-    <row r="107" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G107" s="4"/>
-    </row>
-    <row r="108" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G108" s="4"/>
-    </row>
-    <row r="109" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G109" s="4"/>
-    </row>
-    <row r="110" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G110" s="4"/>
-    </row>
-    <row r="111" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G111" s="4"/>
-    </row>
-    <row r="112" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G112" s="4"/>
-    </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G113" s="4"/>
-    </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G114" s="4"/>
-    </row>
-    <row r="115" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G115" s="4"/>
-    </row>
-    <row r="116" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G116" s="4"/>
-    </row>
-    <row r="117" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G117" s="4"/>
-    </row>
-    <row r="118" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G118" s="4"/>
-    </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G119" s="4"/>
-    </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G120" s="4"/>
-    </row>
-    <row r="121" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G121" s="4"/>
-    </row>
-    <row r="122" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G122" s="4"/>
-    </row>
-    <row r="123" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G123" s="4"/>
-    </row>
-    <row r="124" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G124" s="4"/>
-    </row>
-    <row r="125" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G125" s="4"/>
-    </row>
-    <row r="126" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G126" s="4"/>
-    </row>
-    <row r="127" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G127" s="4"/>
-    </row>
-    <row r="128" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G128" s="4"/>
-    </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G129" s="4"/>
-    </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G130" s="4"/>
-    </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G131" s="4"/>
-    </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G132" s="4"/>
-    </row>
-    <row r="133" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G133" s="4"/>
-    </row>
-    <row r="134" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G134" s="4"/>
-    </row>
-    <row r="135" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G135" s="4"/>
-    </row>
-    <row r="136" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G136" s="4"/>
-    </row>
-    <row r="137" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G137" s="4"/>
-    </row>
-    <row r="138" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G138" s="4"/>
-    </row>
-    <row r="139" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G139" s="4"/>
-    </row>
-    <row r="140" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G140" s="4"/>
-    </row>
-    <row r="141" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G141" s="4"/>
-    </row>
-    <row r="142" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G142" s="4"/>
-    </row>
-    <row r="143" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G143" s="4"/>
-    </row>
-    <row r="144" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G144" s="4"/>
-    </row>
-    <row r="145" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G145" s="4"/>
-    </row>
-    <row r="146" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G146" s="4"/>
-    </row>
-    <row r="147" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G147" s="4"/>
-    </row>
-    <row r="148" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G148" s="4"/>
-    </row>
-    <row r="149" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G149" s="4"/>
-    </row>
-    <row r="150" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G150" s="4"/>
-    </row>
-    <row r="151" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G151" s="4"/>
-    </row>
-    <row r="152" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G152" s="4"/>
-    </row>
-    <row r="153" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G153" s="4"/>
-    </row>
-    <row r="154" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G154" s="4"/>
-    </row>
-    <row r="155" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G155" s="4"/>
-    </row>
-    <row r="156" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G156" s="4"/>
-    </row>
-    <row r="157" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G157" s="4"/>
-    </row>
-    <row r="158" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G158" s="4"/>
-    </row>
-    <row r="159" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G159" s="4"/>
-    </row>
-    <row r="160" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G160" s="4"/>
-    </row>
-    <row r="161" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G161" s="4"/>
-    </row>
-    <row r="162" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G162" s="4"/>
-    </row>
-    <row r="163" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G163" s="4"/>
-    </row>
-    <row r="164" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G164" s="4"/>
-    </row>
-    <row r="165" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G165" s="4"/>
-    </row>
-    <row r="166" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G166" s="4"/>
-    </row>
-    <row r="167" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G167" s="4"/>
-    </row>
-    <row r="168" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G168" s="4"/>
-    </row>
-    <row r="169" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G169" s="4"/>
-    </row>
-    <row r="170" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G170" s="4"/>
-    </row>
-    <row r="171" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G171" s="4"/>
-    </row>
-    <row r="172" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G172" s="4"/>
-    </row>
-    <row r="173" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G173" s="4"/>
-    </row>
-    <row r="174" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G174" s="4"/>
-    </row>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G175" s="4"/>
-    </row>
-    <row r="176" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G176" s="4"/>
-    </row>
-    <row r="177" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G177" s="4"/>
-    </row>
-    <row r="178" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G178" s="4"/>
-    </row>
-    <row r="179" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G179" s="4"/>
-    </row>
-    <row r="180" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G180" s="4"/>
-    </row>
-    <row r="181" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G181" s="4"/>
-    </row>
-    <row r="182" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G182" s="4"/>
-    </row>
-    <row r="183" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G183" s="4"/>
-    </row>
-    <row r="184" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G184" s="4"/>
-    </row>
-    <row r="185" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G185" s="4"/>
-    </row>
-    <row r="186" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G186" s="4"/>
-    </row>
-    <row r="187" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G187" s="4"/>
-    </row>
-    <row r="188" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G188" s="4"/>
-    </row>
-    <row r="189" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G189" s="4"/>
-    </row>
-    <row r="190" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G190" s="4"/>
-    </row>
-    <row r="191" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G191" s="4"/>
-    </row>
-    <row r="192" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G192" s="4"/>
-    </row>
-    <row r="193" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G193" s="4"/>
-    </row>
-    <row r="194" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G194" s="4"/>
-    </row>
-    <row r="195" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G195" s="4"/>
-    </row>
-    <row r="196" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G196" s="4"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H57" s="4"/>
+    </row>
+    <row r="58" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H58" s="4"/>
+    </row>
+    <row r="59" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H59" s="4"/>
+    </row>
+    <row r="60" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H60" s="4"/>
+    </row>
+    <row r="61" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H61" s="4"/>
+    </row>
+    <row r="62" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H63" s="4"/>
+    </row>
+    <row r="64" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H65" s="4"/>
+    </row>
+    <row r="66" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H66" s="4"/>
+    </row>
+    <row r="67" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H67" s="4"/>
+    </row>
+    <row r="68" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H68" s="4"/>
+    </row>
+    <row r="69" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H69" s="4"/>
+    </row>
+    <row r="70" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H70" s="4"/>
+    </row>
+    <row r="71" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H71" s="4"/>
+    </row>
+    <row r="72" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H72" s="4"/>
+    </row>
+    <row r="73" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H73" s="4"/>
+    </row>
+    <row r="74" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H74" s="4"/>
+    </row>
+    <row r="75" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H75" s="4"/>
+    </row>
+    <row r="76" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H76" s="4"/>
+    </row>
+    <row r="77" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H77" s="4"/>
+    </row>
+    <row r="78" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H78" s="4"/>
+    </row>
+    <row r="79" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H79" s="4"/>
+    </row>
+    <row r="80" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H80" s="4"/>
+    </row>
+    <row r="81" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H81" s="4"/>
+    </row>
+    <row r="82" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H82" s="4"/>
+    </row>
+    <row r="83" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H83" s="4"/>
+    </row>
+    <row r="84" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H84" s="4"/>
+    </row>
+    <row r="85" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H85" s="4"/>
+    </row>
+    <row r="86" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H86" s="4"/>
+    </row>
+    <row r="87" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H87" s="4"/>
+    </row>
+    <row r="88" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H88" s="4"/>
+    </row>
+    <row r="89" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H89" s="4"/>
+    </row>
+    <row r="90" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H90" s="4"/>
+    </row>
+    <row r="91" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H91" s="4"/>
+    </row>
+    <row r="92" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H92" s="4"/>
+    </row>
+    <row r="93" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H93" s="4"/>
+    </row>
+    <row r="94" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H94" s="4"/>
+    </row>
+    <row r="95" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H95" s="4"/>
+    </row>
+    <row r="96" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H96" s="4"/>
+    </row>
+    <row r="97" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H97" s="4"/>
+    </row>
+    <row r="98" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H98" s="4"/>
+    </row>
+    <row r="99" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H99" s="4"/>
+    </row>
+    <row r="100" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H100" s="4"/>
+    </row>
+    <row r="101" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H101" s="4"/>
+    </row>
+    <row r="102" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H102" s="4"/>
+    </row>
+    <row r="103" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H103" s="4"/>
+    </row>
+    <row r="104" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H104" s="4"/>
+    </row>
+    <row r="105" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H105" s="4"/>
+    </row>
+    <row r="106" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H106" s="4"/>
+    </row>
+    <row r="107" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H107" s="4"/>
+    </row>
+    <row r="108" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H108" s="4"/>
+    </row>
+    <row r="109" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H109" s="4"/>
+    </row>
+    <row r="110" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H110" s="4"/>
+    </row>
+    <row r="111" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H111" s="4"/>
+    </row>
+    <row r="112" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H112" s="4"/>
+    </row>
+    <row r="113" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H113" s="4"/>
+    </row>
+    <row r="114" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H114" s="4"/>
+    </row>
+    <row r="115" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H115" s="4"/>
+    </row>
+    <row r="116" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H116" s="4"/>
+    </row>
+    <row r="117" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H117" s="4"/>
+    </row>
+    <row r="118" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H118" s="4"/>
+    </row>
+    <row r="119" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H119" s="4"/>
+    </row>
+    <row r="120" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H120" s="4"/>
+    </row>
+    <row r="121" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H121" s="4"/>
+    </row>
+    <row r="122" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H122" s="4"/>
+    </row>
+    <row r="123" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H123" s="4"/>
+    </row>
+    <row r="124" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H124" s="4"/>
+    </row>
+    <row r="125" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H125" s="4"/>
+    </row>
+    <row r="126" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H126" s="4"/>
+    </row>
+    <row r="127" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H127" s="4"/>
+    </row>
+    <row r="128" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H128" s="4"/>
+    </row>
+    <row r="129" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H129" s="4"/>
+    </row>
+    <row r="130" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H130" s="4"/>
+    </row>
+    <row r="131" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H131" s="4"/>
+    </row>
+    <row r="132" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H132" s="4"/>
+    </row>
+    <row r="133" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H133" s="4"/>
+    </row>
+    <row r="134" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H134" s="4"/>
+    </row>
+    <row r="135" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H135" s="4"/>
+    </row>
+    <row r="136" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H136" s="4"/>
+    </row>
+    <row r="137" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H137" s="4"/>
+    </row>
+    <row r="138" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H138" s="4"/>
+    </row>
+    <row r="139" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H139" s="4"/>
+    </row>
+    <row r="140" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H140" s="4"/>
+    </row>
+    <row r="141" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H141" s="4"/>
+    </row>
+    <row r="142" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H142" s="4"/>
+    </row>
+    <row r="143" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H143" s="4"/>
+    </row>
+    <row r="144" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H144" s="4"/>
+    </row>
+    <row r="145" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H145" s="4"/>
+    </row>
+    <row r="146" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H146" s="4"/>
+    </row>
+    <row r="147" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H147" s="4"/>
+    </row>
+    <row r="148" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H148" s="4"/>
+    </row>
+    <row r="149" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H149" s="4"/>
+    </row>
+    <row r="150" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H150" s="4"/>
+    </row>
+    <row r="151" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H151" s="4"/>
+    </row>
+    <row r="152" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H152" s="4"/>
+    </row>
+    <row r="153" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H153" s="4"/>
+    </row>
+    <row r="154" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H154" s="4"/>
+    </row>
+    <row r="155" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H155" s="4"/>
+    </row>
+    <row r="156" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H156" s="4"/>
+    </row>
+    <row r="157" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H157" s="4"/>
+    </row>
+    <row r="158" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H158" s="4"/>
+    </row>
+    <row r="159" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H159" s="4"/>
+    </row>
+    <row r="160" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H160" s="4"/>
+    </row>
+    <row r="161" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H161" s="4"/>
+    </row>
+    <row r="162" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H162" s="4"/>
+    </row>
+    <row r="163" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H163" s="4"/>
+    </row>
+    <row r="164" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H164" s="4"/>
+    </row>
+    <row r="165" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H165" s="4"/>
+    </row>
+    <row r="166" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H166" s="4"/>
+    </row>
+    <row r="167" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H167" s="4"/>
+    </row>
+    <row r="168" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H168" s="4"/>
+    </row>
+    <row r="169" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H169" s="4"/>
+    </row>
+    <row r="170" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H170" s="4"/>
+    </row>
+    <row r="171" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H171" s="4"/>
+    </row>
+    <row r="172" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H172" s="4"/>
+    </row>
+    <row r="173" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H173" s="4"/>
+    </row>
+    <row r="174" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H174" s="4"/>
+    </row>
+    <row r="175" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H175" s="4"/>
+    </row>
+    <row r="176" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H176" s="4"/>
+    </row>
+    <row r="177" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H177" s="4"/>
+    </row>
+    <row r="178" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H178" s="4"/>
+    </row>
+    <row r="179" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H179" s="4"/>
+    </row>
+    <row r="180" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H180" s="4"/>
+    </row>
+    <row r="181" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H181" s="4"/>
+    </row>
+    <row r="182" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H182" s="4"/>
+    </row>
+    <row r="183" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H183" s="4"/>
+    </row>
+    <row r="184" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H184" s="4"/>
+    </row>
+    <row r="185" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H185" s="4"/>
+    </row>
+    <row r="186" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H186" s="4"/>
+    </row>
+    <row r="187" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H187" s="4"/>
+    </row>
+    <row r="188" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H188" s="4"/>
+    </row>
+    <row r="189" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H189" s="4"/>
+    </row>
+    <row r="190" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H190" s="4"/>
+    </row>
+    <row r="191" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H191" s="4"/>
+    </row>
+    <row r="192" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H192" s="4"/>
+    </row>
+    <row r="193" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H193" s="4"/>
+    </row>
+    <row r="194" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H194" s="4"/>
+    </row>
+    <row r="195" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H195" s="4"/>
+    </row>
+    <row r="196" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H196" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A8:J8"/>
+  <autoFilter ref="A8:K8"/>
   <mergeCells count="2">
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="G7:I7"/>
   </mergeCells>
   <pageMargins left="0.11811023622047244" right="0.11811023622047244" top="0.11811023622047244" bottom="0.11811023622047244" header="0" footer="0"/>
   <pageSetup scale="26" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>